<commit_message>
Tanmoy handed to Raja 10.02.2021
</commit_message>
<xml_diff>
--- a/screen_checking.xlsx
+++ b/screen_checking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t xml:space="preserve">Sl.No.</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">Basic Pay must be grater than 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add Branch in employee table</t>
   </si>
 </sst>
 </file>
@@ -58,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -79,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,13 +154,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.92"/>
@@ -214,6 +219,17 @@
       </c>
       <c r="C6" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>